<commit_message>
Updating the Ebios-RM.xlsx file
</commit_message>
<xml_diff>
--- a/Ebios-RM.xlsx
+++ b/Ebios-RM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuentinSIMAR\Desktop\github\EBIOS-RM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DEFEDD3-B3FF-4277-8373-1143EB9D3D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BE6FFA-A097-430B-A7F9-5FD020FD84CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide management risque" sheetId="6" r:id="rId1"/>
@@ -529,12 +529,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF5050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -590,6 +584,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9D05D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB3FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,11 +729,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,46 +741,52 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -793,59 +796,56 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,16 +921,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFB3FF"/>
+      <color rgb="FFFF97FF"/>
+      <color rgb="FFFFC1FF"/>
+      <color rgb="FFFFAFFF"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFF9D05D"/>
       <color rgb="FF00C0BC"/>
       <color rgb="FF00D6D1"/>
       <color rgb="FFB483D9"/>
       <color rgb="FFAA72D4"/>
-      <color rgb="FF001B50"/>
-      <color rgb="FF001132"/>
-      <color rgb="FFFF6D6D"/>
-      <color rgb="FFFFB061"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1404,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B208BB64-555B-43F8-9DA6-D79D99133AD6}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1420,135 +1420,135 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5">
       <c r="A1" s="2"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:6" ht="19.5">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="52" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.5">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="53" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="53" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.5">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="53" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="58"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="1:6" ht="14.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="47" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="58"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="1:6" ht="14.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="58"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="9" spans="1:6" ht="14.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="58"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:6" ht="14.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="59"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1562,7 +1562,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDA11B9-2899-4617-ADB7-E1BD402FD0A3}">
   <sheetPr>
-    <tabColor rgb="FFFFCCFF"/>
+    <tabColor rgb="FFFFB3FF"/>
   </sheetPr>
   <dimension ref="B1:C29"/>
   <sheetViews>
@@ -1714,7 +1714,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17E4CFE-F28E-43CD-B734-6D5BC85C8C1F}">
   <sheetPr>
-    <tabColor rgb="FFFFCCFF"/>
+    <tabColor rgb="FFFFB3FF"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -1816,7 +1816,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85614448-9BE2-4EE8-BEA1-F18EABB3EF4A}">
   <sheetPr>
-    <tabColor rgb="FFFFCCFF"/>
+    <tabColor rgb="FFFFB3FF"/>
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1919,10 +1919,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFB3FF"/>
+  </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1989,6 +1992,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFBB0D2FDE44F94CB78A9106E3FBA332" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="137b1f1cb11a1256ab4a0f5880de417a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="697422ec-95af-4bd2-8276-a0ec7e90a4ab" xmlns:ns3="cdf9ac4b-5435-4bec-af38-1f507fb7cef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daa17bb5a01238db6bf64e5679998ab6" ns2:_="" ns3:_="">
     <xsd:import namespace="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
@@ -2225,15 +2237,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2249,6 +2252,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22357339-C823-4122-A1BF-672EA02855DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2267,14 +2278,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adding the workshop tabs 2
</commit_message>
<xml_diff>
--- a/Ebios-RM.xlsx
+++ b/Ebios-RM.xlsx
@@ -5,21 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuentinSIMAR\Desktop\github\EBIOS-RM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hexgroup-my.sharepoint.com/personal/quentin_simar_hex-group_eu/Documents/Bureau/github/EBIOS-RM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BE6FFA-A097-430B-A7F9-5FD020FD84CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{34FA30CE-0FC9-4941-9723-95B5746A2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5B8001-7465-450C-AAA2-C7A2C1CAE194}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide management risque" sheetId="6" r:id="rId1"/>
     <sheet name="Ateliers" sheetId="7" r:id="rId2"/>
-    <sheet name="Objectifs de l'étude" sheetId="8" r:id="rId3"/>
+    <sheet name="Objectifs de l'étude" sheetId="13" r:id="rId3"/>
     <sheet name="Identification de l'objet" sheetId="4" r:id="rId4"/>
     <sheet name="Mission, valeur métier, bien" sheetId="3" r:id="rId5"/>
     <sheet name="ER, impact, gravité" sheetId="11" r:id="rId6"/>
     <sheet name="Echelle de gravité" sheetId="1" r:id="rId7"/>
+    <sheet name="Socle de sécurité" sheetId="12" r:id="rId8"/>
+    <sheet name="SR_OV" sheetId="14" r:id="rId9"/>
+    <sheet name="SR_OV retenus" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>MISSION</t>
   </si>
@@ -422,6 +425,54 @@
   </si>
   <si>
     <t>CONTEXTE</t>
+  </si>
+  <si>
+    <t>TYPE DE REFERENTIEL</t>
+  </si>
+  <si>
+    <t>NOM DU REFERENTIEL</t>
+  </si>
+  <si>
+    <t>ETAT D'APPLICATION</t>
+  </si>
+  <si>
+    <t>ECARTS</t>
+  </si>
+  <si>
+    <t>JUSTIFICATION DES ECARTS</t>
+  </si>
+  <si>
+    <t>[…]</t>
+  </si>
+  <si>
+    <t>CADRE DE L'ETUDE</t>
+  </si>
+  <si>
+    <t>SOURCES DE RISQUE</t>
+  </si>
+  <si>
+    <t>OBJECTIFS VISES</t>
+  </si>
+  <si>
+    <t>MOTIVATION</t>
+  </si>
+  <si>
+    <t>RESSOURCES</t>
+  </si>
+  <si>
+    <t>ACTIVITE</t>
+  </si>
+  <si>
+    <t>PERTINENCE</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Elevée</t>
+  </si>
+  <si>
+    <t>Faible</t>
   </si>
 </sst>
 </file>
@@ -508,7 +559,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,8 +644,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -715,11 +772,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -796,42 +965,18 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,14 +984,88 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,16 +1140,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF00C0BC"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFF9D05D"/>
+      <color rgb="FFB483D9"/>
+      <color rgb="FFAA72D4"/>
       <color rgb="FFFFB3FF"/>
       <color rgb="FFFF97FF"/>
       <color rgb="FFFFC1FF"/>
       <color rgb="FFFFAFFF"/>
-      <color rgb="FFFF5050"/>
-      <color rgb="FFF9D05D"/>
-      <color rgb="FF00C0BC"/>
       <color rgb="FF00D6D1"/>
-      <color rgb="FFB483D9"/>
-      <color rgb="FFAA72D4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -997,16 +1216,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>557035</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>149063</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2966860</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>53813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1029,7 +1248,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="85725" y="28575"/>
+          <a:off x="4667250" y="4800600"/>
           <a:ext cx="8939035" cy="5464013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1352,210 +1571,303 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E57A49-8761-47D3-B3B1-884E0AA39240}">
-  <dimension ref="B2:B10"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8912F18-1628-4829-BA0F-C664A33B733D}">
+  <sheetPr>
+    <tabColor rgb="FFB483D9"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="1:7" ht="19.5">
+      <c r="A1" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="F5" s="72"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E57A49-8761-47D3-B3B1-884E0AA39240}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.5">
+      <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="42.75">
+      <c r="B3" s="44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="2:2">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="2"/>
-    </row>
+      <c r="C3" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42.75">
+      <c r="B4" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42.75">
+      <c r="B5" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.5">
+      <c r="B6" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5">
+      <c r="B7" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.5">
+      <c r="B8" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" ht="42.75" customHeight="1">
+      <c r="B9" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:6" ht="48" customHeight="1">
+      <c r="B10" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+    </row>
+    <row r="11" spans="1:6" ht="52.5" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B208BB64-555B-43F8-9DA6-D79D99133AD6}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC55D54-C3E6-45AE-B4E7-EA3BA0C1A99E}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" customWidth="1"/>
-    <col min="3" max="3" width="64.140625" customWidth="1"/>
-    <col min="4" max="4" width="68" customWidth="1"/>
-    <col min="5" max="5" width="71.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5">
-      <c r="A1" s="2"/>
-      <c r="B1" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.5">
-      <c r="A2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5">
-      <c r="B3" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="33" customHeight="1">
-      <c r="B4" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.5">
-      <c r="B5" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.25">
-      <c r="B6" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="54"/>
-    </row>
-    <row r="7" spans="1:6" ht="14.25">
-      <c r="B7" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="54"/>
-    </row>
-    <row r="8" spans="1:6" ht="14.25">
-      <c r="B8" s="58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="54"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.25">
-      <c r="B9" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="54"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.25">
-      <c r="B10" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="55"/>
+    <row r="1" spans="1:2">
+      <c r="B1" s="60"/>
+    </row>
+    <row r="2" spans="1:2" ht="19.5">
+      <c r="A2" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1719,7 +2031,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1821,7 +2133,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1852,10 +2164,10 @@
     </row>
     <row r="2" spans="1:6" ht="39.75" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>50</v>
@@ -1866,7 +2178,7 @@
     </row>
     <row r="3" spans="1:6" ht="39.75" customHeight="1">
       <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="20"/>
       <c r="D3" s="8">
         <v>1</v>
@@ -1925,13 +2237,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="98.28515625" customWidth="1"/>
+    <col min="2" max="2" width="99.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5">
@@ -1991,7 +2303,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664BE8FD-FD77-4991-8817-3A56793101DF}">
+  <sheetPr>
+    <tabColor rgb="FFFFB3FF"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5">
+      <c r="A1" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EBC962-3850-43DC-A766-5BF72B128B45}">
+  <sheetPr>
+    <tabColor rgb="FFB483D9"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5">
+      <c r="A1" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2000,7 +2446,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFBB0D2FDE44F94CB78A9106E3FBA332" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="137b1f1cb11a1256ab4a0f5880de417a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="697422ec-95af-4bd2-8276-a0ec7e90a4ab" xmlns:ns3="cdf9ac4b-5435-4bec-af38-1f507fb7cef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daa17bb5a01238db6bf64e5679998ab6" ns2:_="" ns3:_="">
     <xsd:import namespace="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
@@ -2237,21 +2683,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2259,7 +2701,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22357339-C823-4122-A1BF-672EA02855DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2276,14 +2718,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding the workshoptabs 3 & 4
</commit_message>
<xml_diff>
--- a/Ebios-RM.xlsx
+++ b/Ebios-RM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hexgroup-my.sharepoint.com/personal/quentin_simar_hex-group_eu/Documents/Bureau/github/EBIOS-RM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{34FA30CE-0FC9-4941-9723-95B5746A2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5B8001-7465-450C-AAA2-C7A2C1CAE194}"/>
+  <xr:revisionPtr revIDLastSave="537" documentId="13_ncr:1_{34FA30CE-0FC9-4941-9723-95B5746A2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EDFD90A-76FD-4A97-85DD-25803C18CCDC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide management risque" sheetId="6" r:id="rId1"/>
@@ -23,6 +23,13 @@
     <sheet name="Socle de sécurité" sheetId="12" r:id="rId8"/>
     <sheet name="SR_OV" sheetId="14" r:id="rId9"/>
     <sheet name="SR_OV retenus" sheetId="15" r:id="rId10"/>
+    <sheet name="Partie prenante" sheetId="16" r:id="rId11"/>
+    <sheet name="Cartographie menace numérique" sheetId="17" r:id="rId12"/>
+    <sheet name="Scénarios stratégiques" sheetId="18" r:id="rId13"/>
+    <sheet name="Synthèse scénarios stratégiques" sheetId="19" r:id="rId14"/>
+    <sheet name="Scénarios opérationnels" sheetId="20" r:id="rId15"/>
+    <sheet name="Vraisemblance op" sheetId="21" r:id="rId16"/>
+    <sheet name="Echelle vraisemblance op" sheetId="22" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="112">
   <si>
     <t>MISSION</t>
   </si>
@@ -474,12 +481,134 @@
   <si>
     <t>Faible</t>
   </si>
+  <si>
+    <t>CATEGORIE</t>
+  </si>
+  <si>
+    <t>PARTIE PRENANTE</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>C2 - Pharmacie</t>
+  </si>
+  <si>
+    <t>C3 - Clinique privée</t>
+  </si>
+  <si>
+    <t>C1 - Centre hospitalier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE </t>
+  </si>
+  <si>
+    <t>SOURCES DE RISQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEMINS D'ATTAQUE STRATEGIQUES </t>
+  </si>
+  <si>
+    <t>Concurrent</t>
+  </si>
+  <si>
+    <t>Trois chemins d’attaque à investiguer.
+Un concurrent vole des travaux
+de recherche en créant un canal
+d’exfiltration de données :
+1. Portant directement sur le système d'information de la R&amp;D;
+2. Sur le système d’information du laboratoire (P3), qui détient une partie des travaux ;
+3. Passant par le prestataire informatique F3;</t>
+  </si>
+  <si>
+    <t>3 Grave</t>
+  </si>
+  <si>
+    <t>4 Critique</t>
+  </si>
+  <si>
+    <t>Hacktiviste</t>
+  </si>
+  <si>
+    <t>Voler des informations en espionnant les travaux de R&amp;D en vue d’obtenir un avantage concurrentiel</t>
+  </si>
+  <si>
+    <t>Saboter la prochaine campagne nationale de vaccination pour générer un choc psychologique sur la population et discréditer les pouvoirs publics</t>
+  </si>
+  <si>
+    <t>Deux chemins d’attaque à investiguer. Un hacktiviste perturbe la
+production ou la distribution de vaccins :
+1. en provoquant un arrêt de la production industrielle par compromission de l’équipement
+de maintenance du fournisseur de matériel F2 ;
+2. en modifiant l’étiquetage des vaccins.</t>
+  </si>
+  <si>
+    <t>V4 Quasi certain</t>
+  </si>
+  <si>
+    <t>V3 Très vraisemblable</t>
+  </si>
+  <si>
+    <t>V2 Vraisemblable</t>
+  </si>
+  <si>
+    <t>V1 Peu vraisemblable</t>
+  </si>
+  <si>
+    <t>La source de risque va certainement atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est très élevée.</t>
+  </si>
+  <si>
+    <t>La source de risque va probablement atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est élevée.</t>
+  </si>
+  <si>
+    <t>La source de risque est susceptible d’atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est significative.</t>
+  </si>
+  <si>
+    <t>La source de risque a peu de chance d’atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est faible.</t>
+  </si>
+  <si>
+    <t>CHEMINS D'ATTAQUE STRATEGIQUES</t>
+  </si>
+  <si>
+    <t>VRAISSEMBLANCE GLOBALE</t>
+  </si>
+  <si>
+    <t>Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données portant directement sur le système
+d’information de la R&amp;D.</t>
+  </si>
+  <si>
+    <t>Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données sur le système d’information du laboratoire,
+qui détient une partie des travaux.</t>
+  </si>
+  <si>
+    <t>V2 Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données passant par le prestataire informatique.</t>
+  </si>
+  <si>
+    <t>Un hacktiviste perturbe la production de vaccins en provoquant
+un arrêt de la production industrielle par compromission de
+l’équipement de maintenance du fournisseur de matériel.</t>
+  </si>
+  <si>
+    <t>Un hacktiviste perturbe la distribution de vaccins en modifiant
+leur étiquetage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -558,8 +687,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Ubuntu Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Ubuntu Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,8 +791,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDB109"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -876,19 +1053,50 @@
         <color theme="0"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
       <top style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -971,9 +1179,6 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -992,15 +1197,9 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1010,9 +1209,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1023,9 +1219,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1044,28 +1237,113 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,16 +1418,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFEDB109"/>
+      <color rgb="FFF9D05D"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FF00C0BC"/>
-      <color rgb="FFFF5050"/>
-      <color rgb="FFF9D05D"/>
+      <color rgb="FFFBF579"/>
       <color rgb="FFB483D9"/>
       <color rgb="FFAA72D4"/>
       <color rgb="FFFFB3FF"/>
       <color rgb="FFFF97FF"/>
       <color rgb="FFFFC1FF"/>
-      <color rgb="FFFFAFFF"/>
-      <color rgb="FF00D6D1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1217,15 +1495,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>438150</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2966860</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>53813</xdr:rowOff>
+      <xdr:colOff>2985910</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>63338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1248,8 +1526,199 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4667250" y="4800600"/>
+          <a:off x="4686300" y="5295900"/>
           <a:ext cx="8939035" cy="5464013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>7733</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D95261F-50C9-49BA-AEE1-3DAA4E63913E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="627529" y="235323"/>
+          <a:ext cx="7620000" cy="7616528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>232248</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F399186A-99F4-4257-8744-4A0C62B4AF7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="680358"/>
+          <a:ext cx="13186248" cy="6667500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>166353</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>66196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7FB2F37-D7B3-44BC-8E99-29BC7A386A49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13852072" y="761999"/>
+          <a:ext cx="12222281" cy="6325483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156322</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>80632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19ED2231-9D00-4226-9260-604E9425CEE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="918322" y="336176"/>
+          <a:ext cx="9126224" cy="7431691"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1578,8 +2047,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1593,88 +2062,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="67" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="62" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="63" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="74"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="F5" s="72"/>
+      <c r="F5" s="64"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6518065-9EA9-4840-9E69-7D5AA6109689}">
+  <sheetPr>
+    <tabColor rgb="FF00C0BC"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19.5">
+      <c r="A1" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="65"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="78"/>
+      <c r="B3" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="65"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="78"/>
+      <c r="B4" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="65"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A8D408-827F-4799-B4DC-8DD92866F29D}">
+  <sheetPr>
+    <tabColor rgb="FF00C0BC"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AF23-71B2-4A73-BF02-F00BC76BAB48}">
+  <sheetPr>
+    <tabColor rgb="FF00C0BC"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X48" sqref="X48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F25EBB-2D4F-48E3-B33E-71B060A98C1E}">
+  <sheetPr>
+    <tabColor rgb="FF00C0BC"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="80.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19.5">
+      <c r="A1" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="115.5">
+      <c r="A2" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="82.5">
+      <c r="A3" s="83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A4" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="83" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D340FA-0B8A-45F5-B193-2FADB38C7B4E}">
+  <sheetPr>
+    <tabColor rgb="FFEDB109"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3201A9C4-128A-4759-8CAC-DF99B0CAFF27}">
+  <sheetPr>
+    <tabColor rgb="FFEDB109"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5">
+      <c r="A1" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="75.75" customHeight="1">
+      <c r="A2" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="65.25" customHeight="1">
+      <c r="A3" s="98" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="69" customHeight="1">
+      <c r="A4" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="72.75" customHeight="1">
+      <c r="A5" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="61.5" customHeight="1">
+      <c r="A6" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D969813-EC02-488D-AA6D-574B8A4A77A1}">
+  <sheetPr>
+    <tabColor rgb="FFEDB109"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5">
+      <c r="A1" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="75.75" customHeight="1">
+      <c r="A2" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="65.25" customHeight="1">
+      <c r="A3" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="103.5" customHeight="1">
+      <c r="A4" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="89" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="89.25" customHeight="1">
+      <c r="A5" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1686,7 +2498,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1701,19 +2513,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5">
       <c r="A1" s="2"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:6" ht="19.5">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="38" t="s">
@@ -1722,114 +2534,114 @@
       <c r="D2" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="42.75">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="46" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="42.75">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="46" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="42.75">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="46" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.5">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" ht="28.5">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="46" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6" ht="28.5">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="50"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6" ht="42.75" customHeight="1">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6" ht="48" customHeight="1">
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="54"/>
     </row>
     <row r="11" spans="1:6" ht="52.5" customHeight="1"/>
   </sheetData>
@@ -1856,13 +2668,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="60"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" ht="19.5">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="56" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2311,7 +3123,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2323,47 +3135,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="58" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="59" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="64" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="59" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2385,7 +3197,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2395,26 +3207,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="67" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="61" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="59" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2424,29 +3236,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFBB0D2FDE44F94CB78A9106E3FBA332" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="137b1f1cb11a1256ab4a0f5880de417a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="697422ec-95af-4bd2-8276-a0ec7e90a4ab" xmlns:ns3="cdf9ac4b-5435-4bec-af38-1f507fb7cef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daa17bb5a01238db6bf64e5679998ab6" ns2:_="" ns3:_="">
     <xsd:import namespace="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
@@ -2683,25 +3472,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22357339-C823-4122-A1BF-672EA02855DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2718,4 +3512,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout de l'atelier 5
</commit_message>
<xml_diff>
--- a/Ebios-RM.xlsx
+++ b/Ebios-RM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hexgroup-my.sharepoint.com/personal/quentin_simar_hex-group_eu/Documents/Bureau/github/EBIOS-RM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="537" documentId="13_ncr:1_{34FA30CE-0FC9-4941-9723-95B5746A2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EDFD90A-76FD-4A97-85DD-25803C18CCDC}"/>
+  <xr:revisionPtr revIDLastSave="752" documentId="13_ncr:1_{34FA30CE-0FC9-4941-9723-95B5746A2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DEFD4FB-767E-43B0-BDE2-89D213F02CA2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide management risque" sheetId="6" r:id="rId1"/>
@@ -30,6 +30,10 @@
     <sheet name="Scénarios opérationnels" sheetId="20" r:id="rId15"/>
     <sheet name="Vraisemblance op" sheetId="21" r:id="rId16"/>
     <sheet name="Echelle vraisemblance op" sheetId="22" r:id="rId17"/>
+    <sheet name="Synthèse scénarios de risque" sheetId="23" r:id="rId18"/>
+    <sheet name="Stratégie traitement + mesure" sheetId="24" r:id="rId19"/>
+    <sheet name="Mesures de sécurité" sheetId="25" r:id="rId20"/>
+    <sheet name="RR" sheetId="26" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
   <si>
     <t>MISSION</t>
   </si>
@@ -602,6 +606,103 @@
   <si>
     <t>Un hacktiviste perturbe la distribution de vaccins en modifiant
 leur étiquetage</t>
+  </si>
+  <si>
+    <t>NIVEAU DE RISQUE</t>
+  </si>
+  <si>
+    <t>ACCEPTABILITE DU RISQUE</t>
+  </si>
+  <si>
+    <t>INTITULE DES DECISIONS ET DES ACTIONS</t>
+  </si>
+  <si>
+    <t>Moyen</t>
+  </si>
+  <si>
+    <t>Elevé</t>
+  </si>
+  <si>
+    <t>Acceptable en l'état</t>
+  </si>
+  <si>
+    <t>Tolérable sous contrôle</t>
+  </si>
+  <si>
+    <t>Inacceptable</t>
+  </si>
+  <si>
+    <t>Aucune action n'est à entreprendre.</t>
+  </si>
+  <si>
+    <t>Un suivi en termes de gestion du risque est à mener et des actions sont à mettre en place dans le cadre d’une amélioration continue sur le moyen et long terme.</t>
+  </si>
+  <si>
+    <t>Des mesures de réduction du risque doivent impérativement être prises à court terme.
+Dans le cas contraire, tout ou partie de l’activité sera refusé.</t>
+  </si>
+  <si>
+    <t>MESURE DE SECURITE</t>
+  </si>
+  <si>
+    <t>SCENARIOS DE RISQUES ASSOCIES</t>
+  </si>
+  <si>
+    <t>RESPONSABLE</t>
+  </si>
+  <si>
+    <t>FREINS ET DIFFICULTES DE MISE EN ŒUVRE</t>
+  </si>
+  <si>
+    <t>COUT / COMPLEXITE</t>
+  </si>
+  <si>
+    <t>ECHEANCE</t>
+  </si>
+  <si>
+    <t>STATUT</t>
+  </si>
+  <si>
+    <t>Catégorie 1</t>
+  </si>
+  <si>
+    <t>Catégorie 2</t>
+  </si>
+  <si>
+    <t>RR01 - LIBELLE DU RISQUE RESIDUEL : [..]</t>
+  </si>
+  <si>
+    <t>Description et analyse du risque résiduel :</t>
+  </si>
+  <si>
+    <t>Evenements redoutés concernés :</t>
+  </si>
+  <si>
+    <t>Mesures de traitement du risque existantes et complémentaires :</t>
+  </si>
+  <si>
+    <t>Evaluation du risque résiduel :</t>
+  </si>
+  <si>
+    <t>Gravité initiale :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravité résiduelle : </t>
+  </si>
+  <si>
+    <t>Vraisemblance initiale :</t>
+  </si>
+  <si>
+    <t>Vraisemblance résiduelle :</t>
+  </si>
+  <si>
+    <t>Niveau de risque initial :</t>
+  </si>
+  <si>
+    <t>Niveau de risque résiduel :</t>
+  </si>
+  <si>
+    <t>Gestion du risque résiduel :</t>
   </si>
 </sst>
 </file>
@@ -739,12 +840,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFDE53"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00C0BC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -770,12 +865,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB483D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9D05D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,8 +916,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F149"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8BA3E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1092,11 +1193,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1106,11 +1242,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1121,46 +1254,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1170,20 +1303,113 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1191,158 +1417,132 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1418,16 +1618,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFF9F149"/>
+      <color rgb="FFF8BA3E"/>
       <color rgb="FFEDB109"/>
+      <color rgb="FFFBF579"/>
+      <color rgb="FF00C0BC"/>
       <color rgb="FFF9D05D"/>
-      <color rgb="FFFF5050"/>
-      <color rgb="FF00C0BC"/>
-      <color rgb="FFFBF579"/>
       <color rgb="FFB483D9"/>
       <color rgb="FFAA72D4"/>
       <color rgb="FFFFB3FF"/>
-      <color rgb="FFFF97FF"/>
-      <color rgb="FFFFC1FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1719,6 +1919,104 @@
         <a:xfrm>
           <a:off x="918322" y="336176"/>
           <a:ext cx="9126224" cy="7431691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>477672</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>192939</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>121062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5678D93-59B0-4BBA-B767-7EE8154361E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="477672" y="341195"/>
+          <a:ext cx="6084222" cy="7627330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>418171</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1984961</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>35569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{059583E1-E751-4BAC-AAE9-C7FE2A0D0FA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="418171" y="1635513"/>
+          <a:ext cx="6306058" cy="7813544"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2033,7 +2331,7 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2048,102 +2346,102 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:7" ht="18.600000000000001">
+      <c r="A1" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="64" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="95" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="F3" s="60" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="69" t="s">
+      <c r="F4" s="66" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="F5" s="64"/>
+      <c r="F5" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2161,59 +2459,59 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:4" ht="18.600000000000001">
+      <c r="A1" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="65"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="62"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="78"/>
-      <c r="B3" s="77" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="78"/>
-      <c r="B4" s="79" t="s">
+      <c r="A4" s="94"/>
+      <c r="B4" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="64"/>
+      <c r="A5" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2230,11 +2528,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2252,7 +2550,7 @@
       <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2267,70 +2565,70 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="80.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:4" ht="18.600000000000001">
+      <c r="A1" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="115.5">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:4" ht="100.8">
+      <c r="A2" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="101" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="82.5">
-      <c r="A3" s="83" t="s">
+    <row r="3" spans="1:4" ht="72">
+      <c r="A3" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="83" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="75" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2351,9 +2649,9 @@
       <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="4" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2368,61 +2666,61 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="71" customWidth="1"/>
-    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:2" ht="18.600000000000001">
+      <c r="A1" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="69" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75.75" customHeight="1">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="86" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="85" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="69" customHeight="1">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="87" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72.75" customHeight="1">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="85" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="61.5" customHeight="1">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="84" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2439,57 +2737,144 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+    <col min="2" max="2" width="72.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:2" ht="18.600000000000001">
+      <c r="A1" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="69" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75.75" customHeight="1">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="81" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="88" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="103.5" customHeight="1">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="81" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="89.25" customHeight="1">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="82" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5D2F2E-87F9-4360-9E35-7F5BEC8FD084}">
+  <sheetPr>
+    <tabColor rgb="FFFF5050"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="67" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D993CD7-4DFC-41E6-A384-3CDE41991988}">
+  <sheetPr>
+    <tabColor rgb="FFFF5050"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="82" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" customWidth="1"/>
+    <col min="3" max="3" width="81.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.600000000000001">
+      <c r="A1" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.399999999999999" customHeight="1">
+      <c r="A2" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="102" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="103" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30">
+      <c r="A4" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="103" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2497,151 +2882,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E57A49-8761-47D3-B3B1-884E0AA39240}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5">
+    <row r="1" spans="1:6" ht="18.600000000000001">
       <c r="A1" s="2"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.5">
-      <c r="A2" s="12" t="s">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001">
+      <c r="A2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="42.75">
-      <c r="B3" s="43" t="s">
+    <row r="3" spans="1:6" ht="41.4">
+      <c r="B3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75">
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="1:6" ht="41.4">
+      <c r="B4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="42.75">
-      <c r="B5" s="43" t="s">
+    <row r="5" spans="1:6" ht="41.4">
+      <c r="B5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.5">
-      <c r="B6" s="43" t="s">
+    <row r="6" spans="1:6" ht="27.6">
+      <c r="B6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="47"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.5">
-      <c r="B7" s="43" t="s">
+      <c r="E6" s="78"/>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="1:6" ht="27.6">
+      <c r="B7" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="45" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="47"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.5">
-      <c r="B8" s="43" t="s">
+      <c r="E7" s="78"/>
+      <c r="F7" s="45"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.6">
+      <c r="B8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="47"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="45"/>
     </row>
     <row r="9" spans="1:6" ht="42.75" customHeight="1">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="47"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:6" ht="48" customHeight="1">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="54"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:6" ht="52.5" customHeight="1"/>
   </sheetData>
@@ -2650,6 +3035,249 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE21890-1516-4F1C-ADD8-4F9EF368713A}">
+  <sheetPr>
+    <tabColor rgb="FFFF5050"/>
+  </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" customWidth="1"/>
+    <col min="4" max="4" width="42.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="37.200000000000003">
+      <c r="A1" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="106" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="107" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="106" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="106" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="106" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15">
+      <c r="A2" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+    </row>
+    <row r="7" spans="1:7" ht="15">
+      <c r="A7" s="108" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="110"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A7:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C83692E-1EC1-48FE-A029-648A924B35D9}">
+  <sheetPr>
+    <tabColor rgb="FFFF5050"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.600000000000001">
+      <c r="A1" s="119" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="111" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="112"/>
+      <c r="C2" s="113"/>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="112"/>
+      <c r="C3" s="113"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="114" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="115"/>
+      <c r="C4" s="116"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="114" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="115"/>
+      <c r="C5" s="116"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="102" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="102" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="118" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="102" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="102" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="114" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="115"/>
+      <c r="C8" s="116"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2661,20 +3289,20 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="55"/>
-    </row>
-    <row r="2" spans="1:2" ht="19.5">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="53"/>
+    </row>
+    <row r="2" spans="1:2" ht="18.600000000000001">
+      <c r="A2" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="54" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2694,86 +3322,86 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="2:3" ht="17.399999999999999">
+      <c r="B1" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="2:3" ht="16.5">
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="2:3" ht="14.4">
+      <c r="B3" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="16.5">
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="2:3" ht="14.4">
+      <c r="B4" s="27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="16.5">
-      <c r="B5" s="28" t="s">
+    <row r="5" spans="2:3" ht="14.4">
+      <c r="B5" s="27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="16.5">
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="2:3" ht="14.4">
+      <c r="B6" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="16.5">
-      <c r="B7" s="28" t="s">
+    <row r="7" spans="2:3" ht="14.4">
+      <c r="B7" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="16.5">
+    <row r="8" spans="2:3" ht="14.4">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="2:3" ht="16.5">
-      <c r="B9" s="32" t="s">
+    <row r="9" spans="2:3" ht="14.4">
+      <c r="B9" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="16.5">
-      <c r="B10" s="29"/>
+    <row r="10" spans="2:3" ht="14.4">
+      <c r="B10" s="28"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:3" ht="16.5">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:3" ht="14.4">
+      <c r="B11" s="32" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="16.5">
-      <c r="B12" s="30"/>
+    <row r="12" spans="2:3" ht="14.4">
+      <c r="B12" s="29"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="2:3" ht="16.5">
-      <c r="B13" s="33" t="s">
+    <row r="13" spans="2:3" ht="14.4">
+      <c r="B13" s="32" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="16.5">
-      <c r="B14" s="30"/>
+    <row r="14" spans="2:3" ht="14.4">
+      <c r="B14" s="29"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="2:3" ht="16.5">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="2:3" ht="14.4">
+      <c r="B15" s="32" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2781,11 +3409,11 @@
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="31"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" ht="16.5">
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="2:3" ht="14.4">
+      <c r="B17" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2793,7 +3421,7 @@
       </c>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="31"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="2:3">
@@ -2843,80 +3471,80 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="84.5703125" customWidth="1"/>
+    <col min="1" max="1" width="84.5546875" customWidth="1"/>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:2" ht="17.399999999999999">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:2" ht="18.600000000000001">
+      <c r="A2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:2" ht="18.600000000000001">
+      <c r="A3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:2" ht="18.600000000000001">
+      <c r="A4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:2" ht="18.600000000000001">
+      <c r="A5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
-      <c r="A6" s="24"/>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="1:2" ht="19.5">
-      <c r="A7" s="21" t="s">
+    <row r="6" spans="1:2" ht="13.8">
+      <c r="A6" s="23"/>
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:2" ht="18.600000000000001">
+      <c r="A7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:2" ht="18.600000000000001">
+      <c r="A8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19.5">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:2" ht="18.600000000000001">
+      <c r="A9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2945,43 +3573,43 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="8" max="8" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="81.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="18.600000000000001">
+      <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="8">
@@ -2989,50 +3617,50 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="9">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="97">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="9">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="97">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="10">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="10">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="11">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="10">
         <v>4</v>
       </c>
     </row>
@@ -3049,56 +3677,56 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="99.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="99.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" ht="18.600000000000001">
+      <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="49.5">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:2" ht="43.2">
+      <c r="A2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="49.5">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:2" ht="43.2">
+      <c r="A3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="49.5">
-      <c r="A4" s="36" t="s">
+    <row r="4" spans="1:2" ht="43.2">
+      <c r="A4" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="49.5">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:2" ht="43.2">
+      <c r="A5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5">
+    <row r="6" spans="1:2" ht="16.8">
       <c r="A6" s="7"/>
       <c r="B6" s="6"/>
     </row>
@@ -3126,56 +3754,56 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="4" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.600000000000001">
+      <c r="A1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="56" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="57" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="59" t="s">
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="57" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3200,33 +3828,33 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:2" ht="18.600000000000001">
+      <c r="A1" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="64" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="59" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="57" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3236,6 +3864,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFBB0D2FDE44F94CB78A9106E3FBA332" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="137b1f1cb11a1256ab4a0f5880de417a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="697422ec-95af-4bd2-8276-a0ec7e90a4ab" xmlns:ns3="cdf9ac4b-5435-4bec-af38-1f507fb7cef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daa17bb5a01238db6bf64e5679998ab6" ns2:_="" ns3:_="">
     <xsd:import namespace="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
@@ -3472,30 +4123,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="697422ec-95af-4bd2-8276-a0ec7e90a4ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22357339-C823-4122-A1BF-672EA02855DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3512,22 +4158,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F09DFB5-5621-4569-A1B8-D17B8BA8581F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E10371-9AC9-4013-9760-8C8E58478A78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="697422ec-95af-4bd2-8276-a0ec7e90a4ab"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>